<commit_message>
update login close igotit popup update choose answer radio, checkbox and input text
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/login_data.xlsx
+++ b/src/test/java/testdata/login_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Test\IGS-LMS_AutoTest_Intellij\src\test\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD508F7E-56FA-46A1-8594-4163518B7B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480B66E5-7C43-474F-83C6-0637827C5986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4912C522-C4F9-46C1-A63B-37A52B1686B1}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>